<commit_message>
update tenra vampire princess format
</commit_message>
<xml_diff>
--- a/tenra-basho/checklist.xlsx
+++ b/tenra-basho/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tenra-basho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{292F7DD4-DEC6-0241-8F76-68972C22E743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33BDA22-CD8A-E14B-B985-B9E383817F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{8043AA8E-0255-2F4B-B651-BD7F5BD57EE3}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>